<commit_message>
added data to the dataset and modified graphs
</commit_message>
<xml_diff>
--- a/1_data/data_irn_individuals.xlsx
+++ b/1_data/data_irn_individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\7. Doctorat\2. Experiments\2_spodoptera_littoralis\intake_rate_experiment\1_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E16BA1-1B79-4AE0-9C82-3B3BE24B829A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5450812F-53F6-4A67-9A8C-D76F251F29F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B9F4CC11-5A9B-429D-9D62-2573521A7389}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3571" uniqueCount="845">
   <si>
     <t>individual_ID</t>
   </si>
@@ -2925,10 +2925,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6CF4CE-91E2-441D-9D8F-F1AD5C9BC03C}">
   <dimension ref="A1:AK401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AA195" sqref="AA195"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6570,6 +6570,9 @@
       <c r="M43">
         <v>103.7</v>
       </c>
+      <c r="N43">
+        <v>27.4</v>
+      </c>
       <c r="O43" t="s">
         <v>3</v>
       </c>
@@ -6724,6 +6727,9 @@
       <c r="M45">
         <v>138.69999999999999</v>
       </c>
+      <c r="N45">
+        <v>26.5</v>
+      </c>
       <c r="O45" t="s">
         <v>3</v>
       </c>
@@ -6878,6 +6884,9 @@
       <c r="M47" t="s">
         <v>823</v>
       </c>
+      <c r="N47" t="s">
+        <v>823</v>
+      </c>
       <c r="O47" t="s">
         <v>3</v>
       </c>
@@ -7029,6 +7038,9 @@
       <c r="M49">
         <v>135.80000000000001</v>
       </c>
+      <c r="N49">
+        <v>37.200000000000003</v>
+      </c>
       <c r="O49" t="s">
         <v>3</v>
       </c>
@@ -7183,6 +7195,9 @@
       <c r="M51">
         <v>233.3</v>
       </c>
+      <c r="N51">
+        <v>60.4</v>
+      </c>
       <c r="O51" t="s">
         <v>3</v>
       </c>
@@ -7337,6 +7352,9 @@
       <c r="M53">
         <v>189.5</v>
       </c>
+      <c r="N53">
+        <v>55.3</v>
+      </c>
       <c r="O53" t="s">
         <v>3</v>
       </c>
@@ -7491,6 +7509,9 @@
       <c r="M55">
         <v>180.9</v>
       </c>
+      <c r="N55">
+        <v>53.5</v>
+      </c>
       <c r="O55" t="s">
         <v>3</v>
       </c>
@@ -7645,6 +7666,9 @@
       <c r="M57">
         <v>155.80000000000001</v>
       </c>
+      <c r="N57">
+        <v>49.4</v>
+      </c>
       <c r="O57" t="s">
         <v>3</v>
       </c>
@@ -7802,6 +7826,9 @@
       <c r="M59">
         <v>225.8</v>
       </c>
+      <c r="N59">
+        <v>76.8</v>
+      </c>
       <c r="O59" t="s">
         <v>3</v>
       </c>
@@ -7959,6 +7986,9 @@
       <c r="M61">
         <v>221.5</v>
       </c>
+      <c r="N61">
+        <v>78.099999999999994</v>
+      </c>
       <c r="O61" t="s">
         <v>3</v>
       </c>
@@ -8113,6 +8143,9 @@
       <c r="M63">
         <v>158.19999999999999</v>
       </c>
+      <c r="N63">
+        <v>55</v>
+      </c>
       <c r="O63" t="s">
         <v>3</v>
       </c>
@@ -8274,6 +8307,9 @@
       <c r="M65">
         <v>218.5</v>
       </c>
+      <c r="N65">
+        <v>59.8</v>
+      </c>
       <c r="O65" t="s">
         <v>3</v>
       </c>
@@ -8434,6 +8470,9 @@
       <c r="M67">
         <v>248.6</v>
       </c>
+      <c r="N67">
+        <v>85.2</v>
+      </c>
       <c r="O67" t="s">
         <v>3</v>
       </c>
@@ -8591,6 +8630,9 @@
       <c r="M69">
         <v>243.8</v>
       </c>
+      <c r="N69">
+        <v>83.5</v>
+      </c>
       <c r="O69" t="s">
         <v>3</v>
       </c>
@@ -8751,6 +8793,9 @@
       <c r="M71">
         <v>256.10000000000002</v>
       </c>
+      <c r="N71">
+        <v>91.3</v>
+      </c>
       <c r="O71" t="s">
         <v>3</v>
       </c>
@@ -8911,6 +8956,9 @@
       <c r="M73">
         <v>242.1</v>
       </c>
+      <c r="N73">
+        <v>72.3</v>
+      </c>
       <c r="O73" t="s">
         <v>3</v>
       </c>
@@ -9074,6 +9122,9 @@
       <c r="M75">
         <v>248.7</v>
       </c>
+      <c r="N75">
+        <v>79.099999999999994</v>
+      </c>
       <c r="O75" t="s">
         <v>3</v>
       </c>
@@ -9237,6 +9288,9 @@
       <c r="M77">
         <v>258.3</v>
       </c>
+      <c r="N77">
+        <v>95.5</v>
+      </c>
       <c r="O77" t="s">
         <v>3</v>
       </c>
@@ -9403,6 +9457,9 @@
       <c r="M79">
         <v>282.5</v>
       </c>
+      <c r="N79">
+        <v>110.5</v>
+      </c>
       <c r="O79" t="s">
         <v>3</v>
       </c>
@@ -9563,6 +9620,9 @@
       <c r="M81">
         <v>214.8</v>
       </c>
+      <c r="N81">
+        <v>85.2</v>
+      </c>
       <c r="O81" t="s">
         <v>3</v>
       </c>
@@ -12851,6 +12911,9 @@
       <c r="AH123">
         <v>0</v>
       </c>
+      <c r="AI123" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A124">
@@ -13002,6 +13065,9 @@
       <c r="AH125">
         <v>0</v>
       </c>
+      <c r="AI125" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="126" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A126">
@@ -13153,6 +13219,9 @@
       <c r="AH127">
         <v>0</v>
       </c>
+      <c r="AI127" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -13304,6 +13373,9 @@
       <c r="AH129">
         <v>0</v>
       </c>
+      <c r="AI129" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="130" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A130">
@@ -14403,6 +14475,9 @@
       <c r="AH143">
         <v>0</v>
       </c>
+      <c r="AI143" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A144">
@@ -14554,6 +14629,9 @@
       <c r="AH145">
         <v>0</v>
       </c>
+      <c r="AI145" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="146" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A146">
@@ -15028,6 +15106,9 @@
       <c r="AH151">
         <v>0</v>
       </c>
+      <c r="AI151" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="152" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A152">
@@ -15837,6 +15918,9 @@
       <c r="AH161">
         <v>0</v>
       </c>
+      <c r="AI161" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162">
@@ -15866,6 +15950,9 @@
       <c r="J162">
         <v>559.29999999999995</v>
       </c>
+      <c r="K162">
+        <v>86.5</v>
+      </c>
       <c r="O162" t="s">
         <v>3</v>
       </c>
@@ -15919,6 +16006,9 @@
       <c r="C163">
         <v>1</v>
       </c>
+      <c r="D163" t="s">
+        <v>832</v>
+      </c>
       <c r="E163">
         <v>120</v>
       </c>
@@ -15937,6 +16027,9 @@
       <c r="J163">
         <v>550.4</v>
       </c>
+      <c r="L163">
+        <v>262.5</v>
+      </c>
       <c r="O163" t="s">
         <v>3</v>
       </c>
@@ -15969,6 +16062,9 @@
       </c>
       <c r="AB163" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD163" s="1">
+        <v>44530</v>
       </c>
       <c r="AE163" s="1">
         <v>44524</v>
@@ -16005,6 +16101,9 @@
       <c r="J164">
         <v>597.5</v>
       </c>
+      <c r="K164">
+        <v>99.5</v>
+      </c>
       <c r="O164" t="s">
         <v>3</v>
       </c>
@@ -16058,6 +16157,9 @@
       <c r="C165">
         <v>1</v>
       </c>
+      <c r="D165" t="s">
+        <v>831</v>
+      </c>
       <c r="E165">
         <v>120</v>
       </c>
@@ -16075,6 +16177,9 @@
       </c>
       <c r="J165">
         <v>400.9</v>
+      </c>
+      <c r="L165">
+        <v>179.5</v>
       </c>
       <c r="O165" t="s">
         <v>3</v>
@@ -16144,6 +16249,9 @@
       <c r="J166">
         <v>488.7</v>
       </c>
+      <c r="K166">
+        <v>72.900000000000006</v>
+      </c>
       <c r="O166" t="s">
         <v>3</v>
       </c>
@@ -16197,6 +16305,9 @@
       <c r="C167">
         <v>1</v>
       </c>
+      <c r="D167" t="s">
+        <v>831</v>
+      </c>
       <c r="E167">
         <v>120</v>
       </c>
@@ -16215,6 +16326,9 @@
       <c r="J167">
         <v>573.20000000000005</v>
       </c>
+      <c r="L167">
+        <v>246.5</v>
+      </c>
       <c r="O167" t="s">
         <v>3</v>
       </c>
@@ -16247,6 +16361,9 @@
       </c>
       <c r="AB167" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD167" s="1">
+        <v>44530</v>
       </c>
       <c r="AE167" s="1">
         <v>44524</v>
@@ -16283,6 +16400,9 @@
       <c r="J168">
         <v>437.4</v>
       </c>
+      <c r="K168">
+        <v>65.3</v>
+      </c>
       <c r="O168" t="s">
         <v>3</v>
       </c>
@@ -16336,6 +16456,9 @@
       <c r="C169">
         <v>1</v>
       </c>
+      <c r="D169" t="s">
+        <v>831</v>
+      </c>
       <c r="E169">
         <v>120</v>
       </c>
@@ -16354,6 +16477,9 @@
       <c r="J169">
         <v>511.7</v>
       </c>
+      <c r="L169">
+        <v>233.1</v>
+      </c>
       <c r="O169" t="s">
         <v>3</v>
       </c>
@@ -16386,6 +16512,9 @@
       </c>
       <c r="AB169" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD169" s="1">
+        <v>44530</v>
       </c>
       <c r="AE169" s="1">
         <v>44524</v>
@@ -16422,6 +16551,9 @@
       <c r="J170">
         <v>765.4</v>
       </c>
+      <c r="K170">
+        <v>127.5</v>
+      </c>
       <c r="O170" t="s">
         <v>3</v>
       </c>
@@ -16475,6 +16607,9 @@
       <c r="C171">
         <v>2</v>
       </c>
+      <c r="D171" t="s">
+        <v>832</v>
+      </c>
       <c r="E171">
         <v>240</v>
       </c>
@@ -16493,6 +16628,9 @@
       <c r="J171">
         <v>579.4</v>
       </c>
+      <c r="L171">
+        <v>282.10000000000002</v>
+      </c>
       <c r="O171" t="s">
         <v>3</v>
       </c>
@@ -16525,6 +16663,9 @@
       </c>
       <c r="AB171" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD171" s="1">
+        <v>44530</v>
       </c>
       <c r="AE171" s="1">
         <v>44524</v>
@@ -16561,6 +16702,9 @@
       <c r="J172">
         <v>627.29999999999995</v>
       </c>
+      <c r="K172">
+        <v>102.5</v>
+      </c>
       <c r="O172" t="s">
         <v>3</v>
       </c>
@@ -16614,6 +16758,9 @@
       <c r="C173">
         <v>2</v>
       </c>
+      <c r="D173" t="s">
+        <v>831</v>
+      </c>
       <c r="E173">
         <v>240</v>
       </c>
@@ -16632,6 +16779,9 @@
       <c r="J173">
         <v>708.4</v>
       </c>
+      <c r="L173">
+        <v>296.5</v>
+      </c>
       <c r="O173" t="s">
         <v>3</v>
       </c>
@@ -16664,6 +16814,9 @@
       </c>
       <c r="AB173" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD173" s="1">
+        <v>44531</v>
       </c>
       <c r="AE173" s="1">
         <v>44524</v>
@@ -16700,6 +16853,9 @@
       <c r="J174">
         <v>802.5</v>
       </c>
+      <c r="K174">
+        <v>129</v>
+      </c>
       <c r="O174" t="s">
         <v>3</v>
       </c>
@@ -16753,6 +16909,9 @@
       <c r="C175">
         <v>2</v>
       </c>
+      <c r="D175" t="s">
+        <v>831</v>
+      </c>
       <c r="E175">
         <v>240</v>
       </c>
@@ -16771,6 +16930,9 @@
       <c r="J175">
         <v>754.3</v>
       </c>
+      <c r="L175">
+        <v>319.89999999999998</v>
+      </c>
       <c r="O175" t="s">
         <v>3</v>
       </c>
@@ -16803,6 +16965,9 @@
       </c>
       <c r="AB175" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD175" s="1">
+        <v>44530</v>
       </c>
       <c r="AE175" s="1">
         <v>44524</v>
@@ -16839,6 +17004,9 @@
       <c r="J176">
         <v>623.4</v>
       </c>
+      <c r="K176">
+        <v>96.7</v>
+      </c>
       <c r="O176" t="s">
         <v>3</v>
       </c>
@@ -16892,6 +17060,9 @@
       <c r="C177">
         <v>2</v>
       </c>
+      <c r="D177" t="s">
+        <v>831</v>
+      </c>
       <c r="E177">
         <v>240</v>
       </c>
@@ -16910,6 +17081,9 @@
       <c r="J177">
         <v>721.8</v>
       </c>
+      <c r="L177">
+        <v>312.2</v>
+      </c>
       <c r="O177" t="s">
         <v>3</v>
       </c>
@@ -16942,6 +17116,9 @@
       </c>
       <c r="AB177" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD177" s="1">
+        <v>44530</v>
       </c>
       <c r="AE177" s="1">
         <v>44524</v>
@@ -16978,6 +17155,9 @@
       <c r="J178">
         <v>847.3</v>
       </c>
+      <c r="K178">
+        <v>140.80000000000001</v>
+      </c>
       <c r="O178" t="s">
         <v>3</v>
       </c>
@@ -17031,6 +17211,9 @@
       <c r="C179">
         <v>3</v>
       </c>
+      <c r="D179" t="s">
+        <v>832</v>
+      </c>
       <c r="E179">
         <v>360</v>
       </c>
@@ -17049,6 +17232,9 @@
       <c r="J179">
         <v>607.4</v>
       </c>
+      <c r="L179">
+        <v>326.7</v>
+      </c>
       <c r="O179" t="s">
         <v>3</v>
       </c>
@@ -17084,6 +17270,9 @@
       </c>
       <c r="AC179" s="1">
         <v>44526</v>
+      </c>
+      <c r="AD179" s="1">
+        <v>44529</v>
       </c>
       <c r="AE179" s="1">
         <v>44524</v>
@@ -17120,6 +17309,9 @@
       <c r="J180">
         <v>858.3</v>
       </c>
+      <c r="K180">
+        <v>124.2</v>
+      </c>
       <c r="O180" t="s">
         <v>3</v>
       </c>
@@ -17173,6 +17365,9 @@
       <c r="C181">
         <v>3</v>
       </c>
+      <c r="D181" t="s">
+        <v>831</v>
+      </c>
       <c r="E181">
         <v>360</v>
       </c>
@@ -17191,6 +17386,9 @@
       <c r="J181">
         <v>596.1</v>
       </c>
+      <c r="L181">
+        <v>351.5</v>
+      </c>
       <c r="O181" t="s">
         <v>3</v>
       </c>
@@ -17226,6 +17424,9 @@
       </c>
       <c r="AC181" s="1">
         <v>44526</v>
+      </c>
+      <c r="AD181" s="1">
+        <v>44529</v>
       </c>
       <c r="AE181" s="1">
         <v>44524</v>
@@ -17262,6 +17463,9 @@
       <c r="J182">
         <v>733.2</v>
       </c>
+      <c r="K182">
+        <v>113.1</v>
+      </c>
       <c r="O182" t="s">
         <v>3</v>
       </c>
@@ -17318,6 +17522,9 @@
       <c r="C183">
         <v>3</v>
       </c>
+      <c r="D183" t="s">
+        <v>832</v>
+      </c>
       <c r="E183">
         <v>360</v>
       </c>
@@ -17336,6 +17543,9 @@
       <c r="J183">
         <v>798.4</v>
       </c>
+      <c r="L183">
+        <v>361.6</v>
+      </c>
       <c r="O183" t="s">
         <v>3</v>
       </c>
@@ -17371,6 +17581,9 @@
       </c>
       <c r="AB183" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD183" s="1">
+        <v>44530</v>
       </c>
       <c r="AE183" s="1">
         <v>44524</v>
@@ -17407,6 +17620,9 @@
       <c r="J184">
         <v>878.4</v>
       </c>
+      <c r="K184">
+        <v>143.4</v>
+      </c>
       <c r="O184" t="s">
         <v>3</v>
       </c>
@@ -17460,6 +17676,9 @@
       <c r="C185">
         <v>3</v>
       </c>
+      <c r="D185" t="s">
+        <v>831</v>
+      </c>
       <c r="E185">
         <v>360</v>
       </c>
@@ -17478,6 +17697,9 @@
       <c r="J185">
         <v>693.8</v>
       </c>
+      <c r="L185">
+        <v>321.89999999999998</v>
+      </c>
       <c r="O185" t="s">
         <v>3</v>
       </c>
@@ -17513,6 +17735,9 @@
       </c>
       <c r="AB185" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD185" s="1">
+        <v>44531</v>
       </c>
       <c r="AE185" s="1">
         <v>44524</v>
@@ -17549,6 +17774,9 @@
       <c r="J186">
         <v>740.5</v>
       </c>
+      <c r="K186">
+        <v>117.9</v>
+      </c>
       <c r="O186" t="s">
         <v>3</v>
       </c>
@@ -17605,6 +17833,9 @@
       <c r="C187">
         <v>4</v>
       </c>
+      <c r="D187" t="s">
+        <v>832</v>
+      </c>
       <c r="E187">
         <v>480</v>
       </c>
@@ -17623,6 +17854,9 @@
       <c r="J187">
         <v>775.5</v>
       </c>
+      <c r="L187">
+        <v>339.8</v>
+      </c>
       <c r="O187" t="s">
         <v>3</v>
       </c>
@@ -17658,6 +17892,9 @@
       </c>
       <c r="AB187" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD187" s="1">
+        <v>44530</v>
       </c>
       <c r="AE187" s="1">
         <v>44524</v>
@@ -17694,6 +17931,9 @@
       <c r="J188">
         <v>608.29999999999995</v>
       </c>
+      <c r="K188">
+        <v>107.9</v>
+      </c>
       <c r="O188" t="s">
         <v>3</v>
       </c>
@@ -17753,6 +17993,9 @@
       <c r="C189">
         <v>4</v>
       </c>
+      <c r="D189" t="s">
+        <v>832</v>
+      </c>
       <c r="E189">
         <v>480</v>
       </c>
@@ -17771,6 +18014,9 @@
       <c r="J189">
         <v>771.3</v>
       </c>
+      <c r="L189">
+        <v>377.2</v>
+      </c>
       <c r="O189" t="s">
         <v>3</v>
       </c>
@@ -17806,6 +18052,9 @@
       </c>
       <c r="AB189" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD189" s="1">
+        <v>44530</v>
       </c>
       <c r="AE189" s="1">
         <v>44524</v>
@@ -17842,6 +18091,9 @@
       <c r="J190">
         <v>787.2</v>
       </c>
+      <c r="K190">
+        <v>122.1</v>
+      </c>
       <c r="O190" t="s">
         <v>3</v>
       </c>
@@ -17898,6 +18150,9 @@
       <c r="C191">
         <v>4</v>
       </c>
+      <c r="D191" t="s">
+        <v>831</v>
+      </c>
       <c r="E191">
         <v>480</v>
       </c>
@@ -17916,6 +18171,9 @@
       <c r="J191">
         <v>1002.3</v>
       </c>
+      <c r="L191">
+        <v>420.1</v>
+      </c>
       <c r="O191" t="s">
         <v>3</v>
       </c>
@@ -17948,6 +18206,9 @@
       </c>
       <c r="AB191" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD191" s="1">
+        <v>44530</v>
       </c>
       <c r="AE191" s="1">
         <v>44524</v>
@@ -17984,6 +18245,9 @@
       <c r="J192">
         <v>837.7</v>
       </c>
+      <c r="K192">
+        <v>177.1</v>
+      </c>
       <c r="O192" t="s">
         <v>3</v>
       </c>
@@ -18040,6 +18304,9 @@
       <c r="C193">
         <v>4</v>
       </c>
+      <c r="D193" t="s">
+        <v>832</v>
+      </c>
       <c r="E193">
         <v>480</v>
       </c>
@@ -18058,6 +18325,9 @@
       <c r="J193">
         <v>850</v>
       </c>
+      <c r="L193">
+        <v>365.5</v>
+      </c>
       <c r="O193" t="s">
         <v>3</v>
       </c>
@@ -18093,6 +18363,9 @@
       </c>
       <c r="AB193" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD193" s="1">
+        <v>44530</v>
       </c>
       <c r="AE193" s="1">
         <v>44524</v>
@@ -18129,6 +18402,9 @@
       <c r="J194">
         <v>1048.5</v>
       </c>
+      <c r="K194">
+        <v>157.5</v>
+      </c>
       <c r="O194" t="s">
         <v>3</v>
       </c>
@@ -18185,6 +18461,9 @@
       <c r="C195">
         <v>5</v>
       </c>
+      <c r="D195" t="s">
+        <v>832</v>
+      </c>
       <c r="E195">
         <v>900</v>
       </c>
@@ -18203,6 +18482,9 @@
       <c r="J195">
         <v>984.7</v>
       </c>
+      <c r="L195">
+        <v>374.4</v>
+      </c>
       <c r="O195" t="s">
         <v>3</v>
       </c>
@@ -18238,6 +18520,9 @@
       </c>
       <c r="AB195" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD195" s="1">
+        <v>44530</v>
       </c>
       <c r="AE195" s="1">
         <v>44524</v>
@@ -18274,6 +18559,9 @@
       <c r="J196">
         <v>1286.8</v>
       </c>
+      <c r="K196">
+        <v>211.1</v>
+      </c>
       <c r="O196" t="s">
         <v>3</v>
       </c>
@@ -18330,6 +18618,9 @@
       <c r="C197">
         <v>5</v>
       </c>
+      <c r="D197" t="s">
+        <v>831</v>
+      </c>
       <c r="E197">
         <v>900</v>
       </c>
@@ -18348,6 +18639,9 @@
       <c r="J197">
         <v>1010.2</v>
       </c>
+      <c r="L197">
+        <v>374.2</v>
+      </c>
       <c r="O197" t="s">
         <v>3</v>
       </c>
@@ -18383,6 +18677,9 @@
       </c>
       <c r="AB197" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD197" s="1">
+        <v>44530</v>
       </c>
       <c r="AE197" s="1">
         <v>44524</v>
@@ -18419,6 +18716,9 @@
       <c r="J198">
         <v>1019.7</v>
       </c>
+      <c r="K198">
+        <v>163.4</v>
+      </c>
       <c r="O198" t="s">
         <v>3</v>
       </c>
@@ -18475,6 +18775,9 @@
       <c r="C199">
         <v>5</v>
       </c>
+      <c r="D199" t="s">
+        <v>832</v>
+      </c>
       <c r="E199">
         <v>900</v>
       </c>
@@ -18493,6 +18796,9 @@
       <c r="J199">
         <v>1128.5</v>
       </c>
+      <c r="L199">
+        <v>422.2</v>
+      </c>
       <c r="O199" t="s">
         <v>3</v>
       </c>
@@ -18528,6 +18834,9 @@
       </c>
       <c r="AB199" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD199" s="1">
+        <v>44530</v>
       </c>
       <c r="AE199" s="1">
         <v>44524</v>
@@ -18564,6 +18873,9 @@
       <c r="J200">
         <v>911.6</v>
       </c>
+      <c r="K200">
+        <v>143.5</v>
+      </c>
       <c r="O200" t="s">
         <v>3</v>
       </c>
@@ -18620,6 +18932,9 @@
       <c r="C201">
         <v>5</v>
       </c>
+      <c r="D201" t="s">
+        <v>831</v>
+      </c>
       <c r="E201">
         <v>900</v>
       </c>
@@ -18638,6 +18953,9 @@
       <c r="J201">
         <v>1274.2</v>
       </c>
+      <c r="L201">
+        <v>491.5</v>
+      </c>
       <c r="O201" t="s">
         <v>3</v>
       </c>
@@ -18673,6 +18991,9 @@
       </c>
       <c r="AB201" s="1">
         <v>44523</v>
+      </c>
+      <c r="AD201" s="1">
+        <v>44530</v>
       </c>
       <c r="AE201" s="1">
         <v>44524</v>

</xml_diff>

<commit_message>
started writing functions instead of a single script
</commit_message>
<xml_diff>
--- a/1_data/data_irn_individuals.xlsx
+++ b/1_data/data_irn_individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\7. Doctorat\2. Experiments\2_spodoptera_littoralis\intake_rate_experiment\1_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5450812F-53F6-4A67-9A8C-D76F251F29F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F8760-5C65-4CEC-B1AE-E428B54074B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B9F4CC11-5A9B-429D-9D62-2573521A7389}"/>
   </bookViews>
@@ -2603,12 +2603,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2925,10 +2926,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6CF4CE-91E2-441D-9D8F-F1AD5C9BC03C}">
   <dimension ref="A1:AK401"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomLeft" activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2959,7 @@
     <col min="27" max="27" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="23" bestFit="1" customWidth="1"/>
@@ -3055,7 +3056,7 @@
       <c r="AC1" s="2" t="s">
         <v>827</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="5" t="s">
         <v>828</v>
       </c>
       <c r="AE1" s="2" t="s">
@@ -3145,7 +3146,6 @@
         <v>44495</v>
       </c>
       <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
       <c r="AE2" s="1">
         <v>44496</v>
       </c>
@@ -3313,7 +3313,6 @@
         <v>44495</v>
       </c>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
       <c r="AE4" s="1">
         <v>44496</v>
       </c>
@@ -3479,7 +3478,6 @@
         <v>44495</v>
       </c>
       <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
       <c r="AE6" s="1">
         <v>44496</v>
       </c>
@@ -3647,7 +3645,6 @@
         <v>44495</v>
       </c>
       <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
       <c r="AE8" s="1">
         <v>44496</v>
       </c>
@@ -3817,7 +3814,6 @@
       <c r="AC10" s="1">
         <v>44498</v>
       </c>
-      <c r="AD10" s="1"/>
       <c r="AE10" s="1">
         <v>44496</v>
       </c>
@@ -3985,7 +3981,6 @@
         <v>44495</v>
       </c>
       <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
       <c r="AE12" s="1">
         <v>44496</v>
       </c>
@@ -4155,7 +4150,6 @@
         <v>44495</v>
       </c>
       <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
       <c r="AE14" s="1">
         <v>44496</v>
       </c>
@@ -4323,7 +4317,6 @@
         <v>44495</v>
       </c>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
       <c r="AE16" s="1">
         <v>44496</v>
       </c>
@@ -4493,7 +4486,6 @@
       <c r="AC18" s="1">
         <v>44498</v>
       </c>
-      <c r="AD18" s="1"/>
       <c r="AE18" s="1">
         <v>44496</v>
       </c>
@@ -4663,7 +4655,6 @@
       <c r="AC20" s="1">
         <v>44498</v>
       </c>
-      <c r="AD20" s="1"/>
       <c r="AE20" s="1">
         <v>44496</v>
       </c>
@@ -4830,7 +4821,6 @@
         <v>44495</v>
       </c>
       <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
       <c r="AE22" s="1">
         <v>44496</v>
       </c>
@@ -4998,7 +4988,6 @@
         <v>44495</v>
       </c>
       <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
       <c r="AE24" s="1">
         <v>44496</v>
       </c>
@@ -5170,7 +5159,6 @@
       <c r="AC26" s="1">
         <v>44498</v>
       </c>
-      <c r="AD26" s="1"/>
       <c r="AE26" s="1">
         <v>44496</v>
       </c>
@@ -5340,7 +5328,6 @@
       <c r="AC28" s="1">
         <v>44498</v>
       </c>
-      <c r="AD28" s="1"/>
       <c r="AE28" s="1">
         <v>44496</v>
       </c>
@@ -5510,7 +5497,6 @@
       <c r="AC30" s="1">
         <v>44498</v>
       </c>
-      <c r="AD30" s="1"/>
       <c r="AE30" s="1">
         <v>44496</v>
       </c>
@@ -5678,7 +5664,6 @@
         <v>44495</v>
       </c>
       <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
       <c r="AE32" s="1">
         <v>44496</v>
       </c>
@@ -5848,7 +5833,6 @@
       <c r="AC34" s="1">
         <v>44498</v>
       </c>
-      <c r="AD34" s="1"/>
       <c r="AE34" s="1">
         <v>44496</v>
       </c>
@@ -6015,7 +5999,6 @@
       <c r="AB36" s="1">
         <v>44495</v>
       </c>
-      <c r="AD36" s="1"/>
       <c r="AE36" s="1">
         <v>44496</v>
       </c>
@@ -6182,7 +6165,6 @@
       <c r="AB38" s="1">
         <v>44495</v>
       </c>
-      <c r="AD38" s="1"/>
       <c r="AE38" s="1">
         <v>44496</v>
       </c>
@@ -6359,7 +6341,6 @@
       <c r="AC40" s="1">
         <v>44498</v>
       </c>
-      <c r="AD40" s="1"/>
       <c r="AE40" s="1">
         <v>44496</v>
       </c>
@@ -10719,7 +10700,7 @@
       <c r="AB95" s="1">
         <v>44509</v>
       </c>
-      <c r="AD95" t="s">
+      <c r="AD95" s="1" t="s">
         <v>823</v>
       </c>
       <c r="AE95" s="1">

</xml_diff>

<commit_message>
added csv files and finished the load individuals function
</commit_message>
<xml_diff>
--- a/1_data/data_irn_individuals.xlsx
+++ b/1_data/data_irn_individuals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\7. Doctorat\2. Experiments\2_spodoptera_littoralis\intake_rate_experiment\1_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110B88FB-31C8-48D2-8377-E512B43E1C88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC3CF0-1328-46EB-BB6C-BA61FEB837D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B9F4CC11-5A9B-429D-9D62-2573521A7389}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3572" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3571" uniqueCount="845">
   <si>
     <t>individual_ID</t>
   </si>
@@ -2926,10 +2926,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6CF4CE-91E2-441D-9D8F-F1AD5C9BC03C}">
   <dimension ref="A1:AK401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="N155" sqref="N155"/>
+      <selection pane="bottomLeft" activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10721,9 +10721,6 @@
       <c r="AB95" s="1">
         <v>44509</v>
       </c>
-      <c r="AD95" s="1" t="s">
-        <v>823</v>
-      </c>
       <c r="AE95" s="1">
         <v>44510</v>
       </c>

</xml_diff>